<commit_message>
back testing using modified data
</commit_message>
<xml_diff>
--- a/result/201612.xlsx
+++ b/result/201612.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\kra\result\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="120" windowWidth="11655" windowHeight="6030" activeTab="2"/>
+    <workbookView xWindow="9210" yWindow="120" windowWidth="11655" windowHeight="6030" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="3" sheetId="5" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="feature_importance" sheetId="6" r:id="rId4"/>
     <sheet name="20151205" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -381,7 +376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4038,9 +4033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE11" sqref="AE11"/>
+      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8540,8 +8535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8563,7 +8558,7 @@
         <v>76</v>
       </c>
       <c r="F1" s="1">
-        <v>0.38412170000000001</v>
+        <v>0.26245065499999998</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" t="s">
@@ -8788,218 +8783,218 @@
         <v>0.17614798600000001</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1">
-        <v>5.9023509500000002E-2</v>
+        <v>0.16599386699999999</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>0.16599386699999999</v>
       </c>
       <c r="I2" s="1">
-        <v>2.24878326E-2</v>
+        <v>6.1476497599999996E-4</v>
       </c>
       <c r="J2" s="1">
-        <v>4.2911697800000002E-2</v>
+        <v>1.03016424E-3</v>
       </c>
       <c r="K2" s="1">
-        <v>3.4515459300000001E-3</v>
+        <v>5.6644420699999999E-5</v>
       </c>
       <c r="L2" s="1">
-        <v>6.0062723099999996E-3</v>
+        <v>8.0885469599999995E-5</v>
       </c>
       <c r="M2" s="1">
-        <v>1.05174559E-2</v>
+        <v>1.6605117000000001E-4</v>
       </c>
       <c r="N2" s="1">
-        <v>8.2078286099999996E-4</v>
+        <v>2.1151625000000001E-5</v>
       </c>
       <c r="O2" s="1">
-        <v>3.71707973E-3</v>
+        <v>3.0230107999999999E-5</v>
       </c>
       <c r="P2" s="1">
-        <v>8.3504567600000006E-5</v>
+        <v>9.8663581700000002E-7</v>
       </c>
       <c r="Q2" s="1">
-        <v>7.1405844400000001E-3</v>
+        <v>7.6279300300000001E-5</v>
       </c>
       <c r="R2" s="1">
-        <v>6.9015907600000004E-3</v>
+        <v>1.10354249E-4</v>
       </c>
       <c r="S2" s="1">
-        <v>6.9456957600000004E-3</v>
+        <v>1.03855265E-4</v>
       </c>
       <c r="T2" s="1">
-        <v>1.8253366699999999E-2</v>
+        <v>1.3552866599999999E-4</v>
       </c>
       <c r="U2" s="1">
-        <v>5.9023509500000002E-2</v>
+        <v>1.7509510100000001E-4</v>
       </c>
       <c r="V2" s="1">
-        <v>2.0326748700000001E-2</v>
+        <v>9.4164185099999997E-4</v>
       </c>
       <c r="W2" s="1">
-        <v>1.14341809E-2</v>
+        <v>3.6671185299999999E-4</v>
       </c>
       <c r="X2" s="1">
-        <v>1.1193565799999999E-2</v>
+        <v>7.2393263000000002E-4</v>
       </c>
       <c r="Y2" s="1">
-        <v>3.1747289499999998E-2</v>
+        <v>1.9802564799999999E-4</v>
       </c>
       <c r="Z2" s="1">
-        <v>1.5696000299999999E-2</v>
+        <v>2.272946E-4</v>
       </c>
       <c r="AA2" s="1">
-        <v>0.38412170000000001</v>
+        <v>0.26245065499999998</v>
       </c>
       <c r="AB2" s="1">
-        <v>4.81757409E-2</v>
+        <v>0.132606693</v>
       </c>
       <c r="AC2" s="1">
-        <v>2.4756293200000001E-2</v>
+        <v>0.162832749</v>
       </c>
       <c r="AD2" s="1">
-        <v>6.6416023300000003E-3</v>
+        <v>7.1558080199999997E-5</v>
       </c>
       <c r="AE2" s="1">
-        <v>3.5447116499999999E-3</v>
+        <v>2.8373049000000002E-5</v>
       </c>
       <c r="AF2" s="1">
-        <v>1.61428125E-3</v>
+        <v>2.2791314400000001E-5</v>
       </c>
       <c r="AG2" s="1">
-        <v>5.7892078100000004E-4</v>
+        <v>1.67734744E-5</v>
       </c>
       <c r="AH2" s="1">
-        <v>4.39274217E-3</v>
+        <v>6.09036798E-5</v>
       </c>
       <c r="AI2" s="1">
-        <v>1.30372332E-2</v>
+        <v>1.15241431E-4</v>
       </c>
       <c r="AJ2" s="1">
-        <v>8.0283190499999997E-3</v>
+        <v>9.6296799599999996E-5</v>
       </c>
       <c r="AK2" s="1">
-        <v>3.3304760000000002E-3</v>
+        <v>8.8631844600000004E-5</v>
       </c>
       <c r="AL2" s="1">
-        <v>3.4707914699999998E-3</v>
+        <v>1.0176904800000001E-4</v>
       </c>
       <c r="AM2" s="1">
-        <v>2.1489102E-2</v>
+        <v>3.6544163000000002E-4</v>
       </c>
       <c r="AN2" s="1">
-        <v>8.7994205099999993E-3</v>
+        <v>1.3685389499999999E-4</v>
       </c>
       <c r="AO2" s="1">
-        <v>4.9811012E-3</v>
+        <v>1.2653776899999999E-4</v>
       </c>
       <c r="AP2" s="1">
-        <v>5.0671179200000001E-3</v>
+        <v>4.88175435E-5</v>
       </c>
       <c r="AQ2" s="1">
-        <v>2.1277723699999998E-3</v>
+        <v>2.4751457499999999E-5</v>
       </c>
       <c r="AR2" s="1">
-        <v>4.8451265800000002E-3</v>
+        <v>6.1483818800000005E-5</v>
       </c>
       <c r="AS2" s="1">
-        <v>3.7880116999999998E-3</v>
+        <v>6.1383286900000005E-5</v>
       </c>
       <c r="AT2" s="1">
-        <v>3.1000226200000001E-3</v>
+        <v>6.1783204199999996E-5</v>
       </c>
       <c r="AU2" s="1">
-        <v>3.60182606E-3</v>
+        <v>3.9919255899999997E-5</v>
       </c>
       <c r="AV2" s="1">
-        <v>2.9204191499999999E-3</v>
+        <v>2.0848744399999999E-5</v>
       </c>
       <c r="AW2" s="1">
-        <v>2.6773901800000001E-3</v>
+        <v>4.3773611300000002E-5</v>
       </c>
       <c r="AX2" s="1">
-        <v>3.2378252999999998E-3</v>
+        <v>4.92007335E-5</v>
       </c>
       <c r="AY2" s="1">
-        <v>4.8957039100000002E-3</v>
+        <v>5.5665502800000003E-5</v>
       </c>
       <c r="AZ2" s="1">
-        <v>8.6434464699999998E-4</v>
+        <v>1.84230585E-5</v>
       </c>
       <c r="BA2" s="1">
-        <v>1.5793648500000001E-3</v>
+        <v>3.3549694600000002E-5</v>
       </c>
       <c r="BB2" s="1">
-        <v>7.18387373E-3</v>
+        <v>0.117340493</v>
       </c>
       <c r="BC2" s="1">
-        <v>7.9959229400000005E-3</v>
+        <v>0.12772192800000001</v>
       </c>
       <c r="BD2" s="1">
-        <v>1.3004527199999999E-2</v>
+        <v>2.3042249099999999E-2</v>
       </c>
       <c r="BE2" s="1">
-        <v>9.8842238599999993E-3</v>
+        <v>6.2464194300000002E-5</v>
       </c>
       <c r="BF2" s="1">
-        <v>7.65892208E-3</v>
+        <v>4.8358805299999997E-5</v>
       </c>
       <c r="BG2" s="1">
-        <v>5.1130816800000001E-3</v>
+        <v>4.7456839000000003E-5</v>
       </c>
       <c r="BH2" s="1">
-        <v>5.9234333200000001E-3</v>
+        <v>5.0841156999999999E-5</v>
       </c>
       <c r="BI2" s="1">
-        <v>2.9527245299999999E-3</v>
+        <v>4.0578043400000001E-5</v>
       </c>
       <c r="BJ2" s="1">
-        <v>9.8188223799999998E-3</v>
+        <v>9.1799034899999997E-5</v>
       </c>
       <c r="BK2" s="1">
-        <v>6.4799713199999998E-3</v>
+        <v>9.8218392599999996E-5</v>
       </c>
       <c r="BL2" s="1">
-        <v>4.2219373899999996E-3</v>
+        <v>6.8870900599999994E-5</v>
       </c>
       <c r="BM2" s="1">
-        <v>4.6296320099999998E-3</v>
+        <v>7.7394809599999994E-5</v>
       </c>
       <c r="BN2" s="1">
-        <v>3.9191762699999997E-3</v>
+        <v>5.6536225299999999E-5</v>
       </c>
       <c r="BO2" s="1">
-        <v>5.4131067700000004E-3</v>
+        <v>6.4846736299999997E-5</v>
       </c>
       <c r="BP2" s="1">
-        <v>4.3664493000000002E-3</v>
+        <v>5.5626664700000003E-5</v>
       </c>
       <c r="BQ2" s="1">
-        <v>4.1928984600000004E-3</v>
+        <v>4.9991532600000001E-5</v>
       </c>
       <c r="BR2" s="1">
-        <v>4.2919404999999999E-3</v>
+        <v>3.8828314300000002E-5</v>
       </c>
       <c r="BS2" s="1">
-        <v>2.6063061399999999E-3</v>
+        <v>2.2170823099999999E-5</v>
       </c>
       <c r="BT2" s="1">
-        <v>8.2883756700000005E-3</v>
+        <v>8.5614182099999993E-5</v>
       </c>
       <c r="BU2" s="1">
-        <v>6.3079090000000004E-3</v>
+        <v>6.9451634700000005E-5</v>
       </c>
       <c r="BV2" s="1">
-        <v>5.1564653500000002E-3</v>
+        <v>5.9620771900000002E-5</v>
       </c>
       <c r="BW2" s="1">
-        <v>1.25269705E-2</v>
+        <v>6.2991405300000003E-5</v>
       </c>
       <c r="BX2" s="1">
-        <v>3.7372642799999999E-3</v>
+        <v>4.9336844099999997E-5</v>
       </c>
     </row>
     <row r="3" spans="1:76" x14ac:dyDescent="0.3">
@@ -9016,10 +9011,10 @@
         <v>0.162771105</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F3" s="1">
-        <v>4.81757409E-2</v>
+        <v>0.162832749</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -9037,10 +9032,10 @@
         <v>0.12775783499999999</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1">
-        <v>4.2911697800000002E-2</v>
+        <v>0.132606693</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -9058,10 +9053,10 @@
         <v>0.12070434200000001</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1">
-        <v>3.1747289499999998E-2</v>
+        <v>0.12772192800000001</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -9079,10 +9074,10 @@
         <v>0.114430351</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1">
-        <v>2.4756293200000001E-2</v>
+        <v>0.117340493</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -9100,10 +9095,10 @@
         <v>2.3173401199999999E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1">
-        <v>2.24878326E-2</v>
+        <v>2.3042249099999999E-2</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -9121,10 +9116,10 @@
         <v>6.0513058899999998E-4</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1">
-        <v>2.1489102E-2</v>
+        <v>1.03016424E-3</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -9145,7 +9140,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1">
-        <v>2.0326748700000001E-2</v>
+        <v>9.4164185099999997E-4</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -9163,10 +9158,10 @@
         <v>5.4352600000000001E-4</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1">
-        <v>1.8253366699999999E-2</v>
+        <v>7.2393263000000002E-4</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -9184,10 +9179,10 @@
         <v>3.2923351200000002E-4</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1">
-        <v>1.5696000299999999E-2</v>
+        <v>6.1476497599999996E-4</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -9205,10 +9200,10 @@
         <v>2.95335305E-4</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1">
-        <v>1.30372332E-2</v>
+        <v>3.6671185299999999E-4</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -9226,10 +9221,10 @@
         <v>2.0549797499999999E-4</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1">
-        <v>1.3004527199999999E-2</v>
+        <v>3.6544163000000002E-4</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -9247,10 +9242,10 @@
         <v>1.8891860499999999E-4</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1">
-        <v>1.25269705E-2</v>
+        <v>2.272946E-4</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -9268,10 +9263,10 @@
         <v>1.6825190099999999E-4</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1">
-        <v>1.14341809E-2</v>
+        <v>1.9802564799999999E-4</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -9289,10 +9284,10 @@
         <v>1.4648583399999999E-4</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1">
-        <v>1.1193565799999999E-2</v>
+        <v>1.7509510100000001E-4</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -9313,7 +9308,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="1">
-        <v>1.05174559E-2</v>
+        <v>1.6605117000000001E-4</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -9331,10 +9326,10 @@
         <v>1.2250734300000001E-4</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1">
-        <v>9.8842238599999993E-3</v>
+        <v>1.3685389499999999E-4</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -9352,10 +9347,10 @@
         <v>1.17786181E-4</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1">
-        <v>9.8188223799999998E-3</v>
+        <v>1.3552866599999999E-4</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -9373,10 +9368,10 @@
         <v>1.10919163E-4</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F20" s="1">
-        <v>8.7994205099999993E-3</v>
+        <v>1.2653776899999999E-4</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -9394,10 +9389,10 @@
         <v>1.0861653499999999E-4</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="F21" s="1">
-        <v>8.2883756700000005E-3</v>
+        <v>1.15241431E-4</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -9415,10 +9410,10 @@
         <v>1.08039009E-4</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F22" s="1">
-        <v>8.0283190499999997E-3</v>
+        <v>1.10354249E-4</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -9436,10 +9431,10 @@
         <v>1.02342424E-4</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1">
-        <v>7.9959229400000005E-3</v>
+        <v>1.03855265E-4</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -9457,10 +9452,10 @@
         <v>9.3380065300000003E-5</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F24" s="1">
-        <v>7.65892208E-3</v>
+        <v>1.0176904800000001E-4</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -9478,10 +9473,10 @@
         <v>9.0011028699999994E-5</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F25" s="1">
-        <v>7.18387373E-3</v>
+        <v>9.8218392599999996E-5</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -9499,10 +9494,10 @@
         <v>8.5312810399999994E-5</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F26" s="1">
-        <v>7.1405844400000001E-3</v>
+        <v>9.6296799599999996E-5</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -9520,10 +9515,10 @@
         <v>8.3051561299999998E-5</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="F27" s="1">
-        <v>6.9456957600000004E-3</v>
+        <v>9.1799034899999997E-5</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -9541,10 +9536,10 @@
         <v>8.20017516E-5</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F28" s="1">
-        <v>6.9015907600000004E-3</v>
+        <v>8.8631844600000004E-5</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -9562,10 +9557,10 @@
         <v>8.0906302300000002E-5</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F29" s="1">
-        <v>6.6416023300000003E-3</v>
+        <v>8.5614182099999993E-5</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -9583,10 +9578,10 @@
         <v>7.83812684E-5</v>
       </c>
       <c r="E30" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1">
-        <v>6.4799713199999998E-3</v>
+        <v>8.0885469599999995E-5</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -9604,10 +9599,10 @@
         <v>7.35169089E-5</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F31" s="1">
-        <v>6.3079090000000004E-3</v>
+        <v>7.7394809599999994E-5</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -9625,10 +9620,10 @@
         <v>6.9079728900000003E-5</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F32" s="1">
-        <v>6.0062723099999996E-3</v>
+        <v>7.6279300300000001E-5</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -9646,10 +9641,10 @@
         <v>6.6486989800000005E-5</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="F33" s="1">
-        <v>5.9234333200000001E-3</v>
+        <v>7.1558080199999997E-5</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -9667,10 +9662,10 @@
         <v>6.3536800100000003E-5</v>
       </c>
       <c r="E34" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F34" s="1">
-        <v>5.4131067700000004E-3</v>
+        <v>6.9451634700000005E-5</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -9688,10 +9683,10 @@
         <v>6.1487819299999998E-5</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F35" s="1">
-        <v>5.1564653500000002E-3</v>
+        <v>6.8870900599999994E-5</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -9709,10 +9704,10 @@
         <v>6.0579933100000001E-5</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F36" s="1">
-        <v>5.1130816800000001E-3</v>
+        <v>6.4846736299999997E-5</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -9730,10 +9725,10 @@
         <v>6.0480359499999997E-5</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F37" s="1">
-        <v>5.0671179200000001E-3</v>
+        <v>6.2991405300000003E-5</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -9751,10 +9746,10 @@
         <v>5.7479761600000001E-5</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F38" s="1">
-        <v>4.9811012E-3</v>
+        <v>6.2464194300000002E-5</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -9772,10 +9767,10 @@
         <v>5.7157809400000001E-5</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F39" s="1">
-        <v>4.8957039100000002E-3</v>
+        <v>6.1783204199999996E-5</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -9796,7 +9791,7 @@
         <v>41</v>
       </c>
       <c r="F40" s="1">
-        <v>4.8451265800000002E-3</v>
+        <v>6.1483818800000005E-5</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -9814,10 +9809,10 @@
         <v>5.59872968E-5</v>
       </c>
       <c r="E41" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="F41" s="1">
-        <v>4.6296320099999998E-3</v>
+        <v>6.1383286900000005E-5</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -9838,7 +9833,7 @@
         <v>31</v>
       </c>
       <c r="F42" s="1">
-        <v>4.39274217E-3</v>
+        <v>6.09036798E-5</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -9856,10 +9851,10 @@
         <v>5.5713743799999999E-5</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F43" s="1">
-        <v>4.3664493000000002E-3</v>
+        <v>5.9620771900000002E-5</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -9877,10 +9872,10 @@
         <v>5.5600129800000002E-5</v>
       </c>
       <c r="E44" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1">
-        <v>4.2919404999999999E-3</v>
+        <v>5.6644420699999999E-5</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -9898,10 +9893,10 @@
         <v>5.3687147399999998E-5</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F45" s="1">
-        <v>4.2219373899999996E-3</v>
+        <v>5.6536225299999999E-5</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -9919,10 +9914,10 @@
         <v>5.2301202200000002E-5</v>
       </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F46" s="1">
-        <v>4.1928984600000004E-3</v>
+        <v>5.5665502800000003E-5</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -9940,10 +9935,10 @@
         <v>5.1137526999999997E-5</v>
       </c>
       <c r="E47" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F47" s="1">
-        <v>3.9191762699999997E-3</v>
+        <v>5.5626664700000003E-5</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -9961,10 +9956,10 @@
         <v>4.9284146799999997E-5</v>
       </c>
       <c r="E48" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F48" s="1">
-        <v>3.7880116999999998E-3</v>
+        <v>5.0841156999999999E-5</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -9982,10 +9977,10 @@
         <v>4.82633438E-5</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F49" s="1">
-        <v>3.7372642799999999E-3</v>
+        <v>4.9991532600000001E-5</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -10003,10 +9998,10 @@
         <v>4.70544796E-5</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="F50" s="1">
-        <v>3.71707973E-3</v>
+        <v>4.9336844099999997E-5</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -10024,10 +10019,10 @@
         <v>4.6688983E-5</v>
       </c>
       <c r="E51" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F51" s="1">
-        <v>3.60182606E-3</v>
+        <v>4.92007335E-5</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -10045,10 +10040,10 @@
         <v>4.6328468499999999E-5</v>
       </c>
       <c r="E52" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F52" s="1">
-        <v>3.5447116499999999E-3</v>
+        <v>4.88175435E-5</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -10066,10 +10061,10 @@
         <v>4.4265511700000003E-5</v>
       </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F53" s="1">
-        <v>3.4707914699999998E-3</v>
+        <v>4.8358805299999997E-5</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -10087,10 +10082,10 @@
         <v>4.3532468999999999E-5</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F54" s="1">
-        <v>3.4515459300000001E-3</v>
+        <v>4.7456839000000003E-5</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -10108,10 +10103,10 @@
         <v>4.2121927099999999E-5</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F55" s="1">
-        <v>3.3304760000000002E-3</v>
+        <v>4.3773611300000002E-5</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -10129,10 +10124,10 @@
         <v>3.7944449699999997E-5</v>
       </c>
       <c r="E56" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F56" s="1">
-        <v>3.2378252999999998E-3</v>
+        <v>4.0578043400000001E-5</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -10150,10 +10145,10 @@
         <v>3.7429067E-5</v>
       </c>
       <c r="E57" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F57" s="1">
-        <v>3.1000226200000001E-3</v>
+        <v>3.9919255899999997E-5</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -10171,10 +10166,10 @@
         <v>3.1804179200000002E-5</v>
       </c>
       <c r="E58" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F58" s="1">
-        <v>2.9527245299999999E-3</v>
+        <v>3.8828314300000002E-5</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -10192,10 +10187,10 @@
         <v>2.9836405000000002E-5</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F59" s="1">
-        <v>2.9204191499999999E-3</v>
+        <v>3.3549694600000002E-5</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -10213,10 +10208,10 @@
         <v>2.4399308299999999E-5</v>
       </c>
       <c r="E60" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F60" s="1">
-        <v>2.6773901800000001E-3</v>
+        <v>3.0230107999999999E-5</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -10234,10 +10229,10 @@
         <v>2.35950108E-5</v>
       </c>
       <c r="E61" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="F61" s="1">
-        <v>2.6063061399999999E-3</v>
+        <v>2.8373049000000002E-5</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -10258,7 +10253,7 @@
         <v>40</v>
       </c>
       <c r="F62" s="1">
-        <v>2.1277723699999998E-3</v>
+        <v>2.4751457499999999E-5</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -10279,7 +10274,7 @@
         <v>29</v>
       </c>
       <c r="F63" s="1">
-        <v>1.61428125E-3</v>
+        <v>2.2791314400000001E-5</v>
       </c>
       <c r="G63" s="1"/>
     </row>
@@ -10297,10 +10292,10 @@
         <v>1.8515246299999999E-5</v>
       </c>
       <c r="E64" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="F64" s="1">
-        <v>1.5793648500000001E-3</v>
+        <v>2.2170823099999999E-5</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -10318,10 +10313,10 @@
         <v>1.7227976199999999E-5</v>
       </c>
       <c r="E65" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F65" s="1">
-        <v>8.6434464699999998E-4</v>
+        <v>2.1151625000000001E-5</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -10339,10 +10334,10 @@
         <v>1.6698310500000001E-5</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F66" s="1">
-        <v>8.2078286099999996E-4</v>
+        <v>2.0848744399999999E-5</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -10354,10 +10349,10 @@
         <v>1.5701056299999999E-5</v>
       </c>
       <c r="E67" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F67" s="1">
-        <v>5.7892078100000004E-4</v>
+        <v>1.84230585E-5</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -10368,10 +10363,10 @@
         <v>1.5588980600000001E-5</v>
       </c>
       <c r="E68" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F68" s="1">
-        <v>8.3504567600000006E-5</v>
+        <v>1.67734744E-5</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -10382,10 +10377,10 @@
         <v>9.9243465900000007E-7</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F69" s="1">
-        <v>0</v>
+        <v>9.8663581700000002E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data format change to int back testing..
</commit_message>
<xml_diff>
--- a/result/201612.xlsx
+++ b/result/201612.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\kra\result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="120" windowWidth="11655" windowHeight="6030" activeTab="3"/>
+    <workbookView minimized="1" xWindow="10995" yWindow="120" windowWidth="11655" windowHeight="6030" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="3" sheetId="5" r:id="rId1"/>
     <sheet name="4" sheetId="8" r:id="rId2"/>
     <sheet name="10" sheetId="11" r:id="rId3"/>
-    <sheet name="feature_importance" sheetId="6" r:id="rId4"/>
-    <sheet name="20151205" sheetId="7" r:id="rId5"/>
+    <sheet name="11" sheetId="12" r:id="rId4"/>
+    <sheet name="feature_importance" sheetId="6" r:id="rId5"/>
+    <sheet name="20151205" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="79">
   <si>
     <t>seoul</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -376,7 +382,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +417,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4035,7 +4041,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8533,10 +8539,1157 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.625" customWidth="1"/>
+    <col min="3" max="3" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" customWidth="1"/>
+    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <f>SUM(G2:G300)</f>
+        <v>-626.20000000000005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2">
+        <v>2.1</v>
+      </c>
+      <c r="G2">
+        <f>F2*10-10</f>
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <f>G2+G9+G16+G23+G30+G37+G44+G51+G58+G65+G72+G79</f>
+        <v>-89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>F3*10/3-10</f>
+        <v>-10</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">G3+G10+G17+G24+G31+G38+G45+G52+G59+G66+G73+G80</f>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>F4*10-10</f>
+        <v>-10</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>F5*10/4-10</f>
+        <v>-10</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>12.8</v>
+      </c>
+      <c r="G6">
+        <f>F6*10/10-10</f>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-97.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>F7*10/23-10</f>
+        <v>-10</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9" si="1">F9*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10" si="2">F10*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11" si="3">F11*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12" si="4">F12*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="5">F13*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="6">F14*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16" si="7">F16*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17" si="8">F17*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18" si="9">F18*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19" si="10">F19*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20" si="11">F20*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21" si="12">F21*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23" si="13">F23*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24" si="14">F24*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25" si="15">F25*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26" si="16">F26*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ref="G27" si="17">F27*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28" si="18">F28*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30" si="19">F30*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31" si="20">F31*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32" si="21">F32*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33" si="22">F33*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34" si="23">F34*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35" si="24">F35*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37" si="25">F37*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38" si="26">F38*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39" si="27">F39*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40" si="28">F40*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ref="G41" si="29">F41*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42" si="30">F42*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44" si="31">F44*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45" si="32">F45*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ref="G46" si="33">F46*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47" si="34">F47*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48" si="35">F48*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49" si="36">F49*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ref="G51" si="37">F51*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52" si="38">F52*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ref="G53" si="39">F53*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" ref="G54" si="40">F54*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" ref="G55" si="41">F55*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" ref="G56" si="42">F56*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ref="G58" si="43">F58*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <f t="shared" ref="G59" si="44">F59*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ref="G60" si="45">F60*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <f t="shared" ref="G61" si="46">F61*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ref="G62" si="47">F62*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ref="G63" si="48">F63*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <f t="shared" ref="G65" si="49">F65*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ref="G66" si="50">F66*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67" si="51">F67*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <f t="shared" ref="G68" si="52">F68*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <f t="shared" ref="G69" si="53">F69*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <f t="shared" ref="G70" si="54">F70*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="C72">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>75</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <f t="shared" ref="G72" si="55">F72*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <f t="shared" ref="G73" si="56">F73*10/3-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>3</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <f t="shared" ref="G74" si="57">F74*10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>12</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ref="G75" si="58">F75*10/4-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <f t="shared" ref="G76" si="59">F76*10/10-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <f t="shared" ref="G77" si="60">F77*10/23-10</f>
+        <v>-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8555,10 +9708,10 @@
         <v>0.26884050100000001</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1">
-        <v>0.26245065499999998</v>
+        <v>0.216735821</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" t="s">
@@ -8783,218 +9936,218 @@
         <v>0.17614798600000001</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1">
-        <v>0.16599386699999999</v>
+        <v>6.2739103500000004E-2</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1">
-        <v>0.16599386699999999</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>6.1476497599999996E-4</v>
+        <v>3.35005741E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>1.03016424E-3</v>
+        <v>0.216735821</v>
       </c>
       <c r="K2" s="1">
-        <v>5.6644420699999999E-5</v>
+        <v>4.8479553199999997E-3</v>
       </c>
       <c r="L2" s="1">
-        <v>8.0885469599999995E-5</v>
+        <v>8.7234240200000004E-3</v>
       </c>
       <c r="M2" s="1">
-        <v>1.6605117000000001E-4</v>
+        <v>1.7387763099999998E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>2.1151625000000001E-5</v>
+        <v>3.1657826199999999E-3</v>
       </c>
       <c r="O2" s="1">
-        <v>3.0230107999999999E-5</v>
+        <v>3.30297449E-3</v>
       </c>
       <c r="P2" s="1">
-        <v>9.8663581700000002E-7</v>
+        <v>5.8890088800000001E-5</v>
       </c>
       <c r="Q2" s="1">
-        <v>7.6279300300000001E-5</v>
+        <v>1.13727923E-2</v>
       </c>
       <c r="R2" s="1">
-        <v>1.10354249E-4</v>
+        <v>1.2671995599999999E-2</v>
       </c>
       <c r="S2" s="1">
-        <v>1.03855265E-4</v>
+        <v>1.5341451000000001E-2</v>
       </c>
       <c r="T2" s="1">
-        <v>1.3552866599999999E-4</v>
+        <v>5.68563505E-2</v>
       </c>
       <c r="U2" s="1">
-        <v>1.7509510100000001E-4</v>
+        <v>7.9079522999999999E-3</v>
       </c>
       <c r="V2" s="1">
-        <v>9.4164185099999997E-4</v>
+        <v>4.0322352300000003E-2</v>
       </c>
       <c r="W2" s="1">
-        <v>3.6671185299999999E-4</v>
+        <v>1.5826215000000001E-2</v>
       </c>
       <c r="X2" s="1">
-        <v>7.2393263000000002E-4</v>
+        <v>1.20636571E-2</v>
       </c>
       <c r="Y2" s="1">
-        <v>1.9802564799999999E-4</v>
+        <v>1.8757551000000001E-2</v>
       </c>
       <c r="Z2" s="1">
-        <v>2.272946E-4</v>
+        <v>2.4455601600000001E-2</v>
       </c>
       <c r="AA2" s="1">
-        <v>0.26245065499999998</v>
+        <v>1.1553381600000001E-2</v>
       </c>
       <c r="AB2" s="1">
-        <v>0.132606693</v>
+        <v>7.0506677900000004E-3</v>
       </c>
       <c r="AC2" s="1">
-        <v>0.162832749</v>
+        <v>1.2074678E-2</v>
       </c>
       <c r="AD2" s="1">
-        <v>7.1558080199999997E-5</v>
+        <v>1.8819608500000001E-2</v>
       </c>
       <c r="AE2" s="1">
-        <v>2.8373049000000002E-5</v>
+        <v>2.9440972100000001E-3</v>
       </c>
       <c r="AF2" s="1">
-        <v>2.2791314400000001E-5</v>
+        <v>3.4321147799999999E-3</v>
       </c>
       <c r="AG2" s="1">
-        <v>1.67734744E-5</v>
+        <v>5.3064338699999999E-4</v>
       </c>
       <c r="AH2" s="1">
-        <v>6.09036798E-5</v>
+        <v>6.6078185100000002E-3</v>
       </c>
       <c r="AI2" s="1">
-        <v>1.15241431E-4</v>
+        <v>2.1383888300000001E-2</v>
       </c>
       <c r="AJ2" s="1">
-        <v>9.6296799599999996E-5</v>
+        <v>1.1879538E-2</v>
       </c>
       <c r="AK2" s="1">
-        <v>8.8631844600000004E-5</v>
+        <v>4.5794539400000004E-3</v>
       </c>
       <c r="AL2" s="1">
-        <v>1.0176904800000001E-4</v>
+        <v>4.2988041200000002E-3</v>
       </c>
       <c r="AM2" s="1">
-        <v>3.6544163000000002E-4</v>
+        <v>1.9325936299999999E-2</v>
       </c>
       <c r="AN2" s="1">
-        <v>1.3685389499999999E-4</v>
+        <v>1.4422597800000001E-2</v>
       </c>
       <c r="AO2" s="1">
-        <v>1.2653776899999999E-4</v>
+        <v>3.2558153900000002E-3</v>
       </c>
       <c r="AP2" s="1">
-        <v>4.88175435E-5</v>
+        <v>2.85742901E-2</v>
       </c>
       <c r="AQ2" s="1">
-        <v>2.4751457499999999E-5</v>
+        <v>3.5338394499999999E-3</v>
       </c>
       <c r="AR2" s="1">
-        <v>6.1483818800000005E-5</v>
+        <v>6.4394017399999996E-3</v>
       </c>
       <c r="AS2" s="1">
-        <v>6.1383286900000005E-5</v>
+        <v>6.5493793700000004E-3</v>
       </c>
       <c r="AT2" s="1">
-        <v>6.1783204199999996E-5</v>
+        <v>3.6327386599999999E-3</v>
       </c>
       <c r="AU2" s="1">
-        <v>3.9919255899999997E-5</v>
+        <v>2.5420987200000002E-3</v>
       </c>
       <c r="AV2" s="1">
-        <v>2.0848744399999999E-5</v>
+        <v>5.6009470300000001E-3</v>
       </c>
       <c r="AW2" s="1">
-        <v>4.3773611300000002E-5</v>
+        <v>4.12321055E-3</v>
       </c>
       <c r="AX2" s="1">
-        <v>4.92007335E-5</v>
+        <v>5.3857450399999998E-3</v>
       </c>
       <c r="AY2" s="1">
-        <v>5.5665502800000003E-5</v>
+        <v>2.91751204E-3</v>
       </c>
       <c r="AZ2" s="1">
-        <v>1.84230585E-5</v>
+        <v>1.56710392E-3</v>
       </c>
       <c r="BA2" s="1">
-        <v>3.3549694600000002E-5</v>
+        <v>2.1550414900000001E-3</v>
       </c>
       <c r="BB2" s="1">
-        <v>0.117340493</v>
+        <v>1.6445249299999999E-2</v>
       </c>
       <c r="BC2" s="1">
-        <v>0.12772192800000001</v>
+        <v>6.2739103500000004E-2</v>
       </c>
       <c r="BD2" s="1">
-        <v>2.3042249099999999E-2</v>
+        <v>8.1122279500000002E-3</v>
       </c>
       <c r="BE2" s="1">
-        <v>6.2464194300000002E-5</v>
+        <v>1.1062789199999999E-2</v>
       </c>
       <c r="BF2" s="1">
-        <v>4.8358805299999997E-5</v>
+        <v>9.7167137800000004E-3</v>
       </c>
       <c r="BG2" s="1">
-        <v>4.7456839000000003E-5</v>
+        <v>7.4428997E-3</v>
       </c>
       <c r="BH2" s="1">
-        <v>5.0841156999999999E-5</v>
+        <v>7.2607542500000002E-3</v>
       </c>
       <c r="BI2" s="1">
-        <v>4.0578043400000001E-5</v>
+        <v>5.4257679200000004E-3</v>
       </c>
       <c r="BJ2" s="1">
-        <v>9.1799034899999997E-5</v>
+        <v>1.29081903E-2</v>
       </c>
       <c r="BK2" s="1">
-        <v>9.8218392599999996E-5</v>
+        <v>1.11576683E-2</v>
       </c>
       <c r="BL2" s="1">
-        <v>6.8870900599999994E-5</v>
+        <v>8.2916871699999992E-3</v>
       </c>
       <c r="BM2" s="1">
-        <v>7.7394809599999994E-5</v>
+        <v>9.9446641799999999E-3</v>
       </c>
       <c r="BN2" s="1">
-        <v>5.6536225299999999E-5</v>
+        <v>8.3742176800000005E-3</v>
       </c>
       <c r="BO2" s="1">
-        <v>6.4846736299999997E-5</v>
+        <v>8.6156411100000007E-3</v>
       </c>
       <c r="BP2" s="1">
-        <v>5.5626664700000003E-5</v>
+        <v>1.03199963E-2</v>
       </c>
       <c r="BQ2" s="1">
-        <v>4.9991532600000001E-5</v>
+        <v>8.6318010399999996E-3</v>
       </c>
       <c r="BR2" s="1">
-        <v>3.8828314300000002E-5</v>
+        <v>8.61218253E-3</v>
       </c>
       <c r="BS2" s="1">
-        <v>2.2170823099999999E-5</v>
+        <v>4.7746699200000003E-3</v>
       </c>
       <c r="BT2" s="1">
-        <v>8.5614182099999993E-5</v>
+        <v>1.29375866E-2</v>
       </c>
       <c r="BU2" s="1">
-        <v>6.9451634700000005E-5</v>
+        <v>1.95506729E-2</v>
       </c>
       <c r="BV2" s="1">
-        <v>5.9620771900000002E-5</v>
+        <v>9.6578771000000001E-3</v>
       </c>
       <c r="BW2" s="1">
-        <v>6.2991405300000003E-5</v>
+        <v>1.13898E-2</v>
       </c>
       <c r="BX2" s="1">
-        <v>4.9336844099999997E-5</v>
+        <v>8.1483840399999997E-3</v>
       </c>
     </row>
     <row r="3" spans="1:76" x14ac:dyDescent="0.3">
@@ -9011,10 +10164,10 @@
         <v>0.162771105</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1">
-        <v>0.162832749</v>
+        <v>5.68563505E-2</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -9032,10 +10185,10 @@
         <v>0.12775783499999999</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1">
-        <v>0.132606693</v>
+        <v>4.0322352300000003E-2</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -9053,10 +10206,10 @@
         <v>0.12070434200000001</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1">
-        <v>0.12772192800000001</v>
+        <v>3.35005741E-2</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -9074,10 +10227,10 @@
         <v>0.114430351</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1">
-        <v>0.117340493</v>
+        <v>2.85742901E-2</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -9095,10 +10248,10 @@
         <v>2.3173401199999999E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1">
-        <v>2.3042249099999999E-2</v>
+        <v>2.4455601600000001E-2</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -9116,10 +10269,10 @@
         <v>6.0513058899999998E-4</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
-        <v>1.03016424E-3</v>
+        <v>2.1383888300000001E-2</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -9137,10 +10290,10 @@
         <v>6.0028590800000005E-4</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1">
-        <v>9.4164185099999997E-4</v>
+        <v>1.95506729E-2</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -9158,10 +10311,10 @@
         <v>5.4352600000000001E-4</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1">
-        <v>7.2393263000000002E-4</v>
+        <v>1.9325936299999999E-2</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -9179,10 +10332,10 @@
         <v>3.2923351200000002E-4</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1">
-        <v>6.1476497599999996E-4</v>
+        <v>1.8819608500000001E-2</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -9200,10 +10353,10 @@
         <v>2.95335305E-4</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1">
-        <v>3.6671185299999999E-4</v>
+        <v>1.8757551000000001E-2</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -9221,10 +10374,10 @@
         <v>2.0549797499999999E-4</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1">
-        <v>3.6544163000000002E-4</v>
+        <v>1.7387763099999998E-2</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -9242,10 +10395,10 @@
         <v>1.8891860499999999E-4</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1">
-        <v>2.272946E-4</v>
+        <v>1.6445249299999999E-2</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -9263,10 +10416,10 @@
         <v>1.6825190099999999E-4</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1">
-        <v>1.9802564799999999E-4</v>
+        <v>1.5826215000000001E-2</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -9284,10 +10437,10 @@
         <v>1.4648583399999999E-4</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1">
-        <v>1.7509510100000001E-4</v>
+        <v>1.5341451000000001E-2</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -9305,10 +10458,10 @@
         <v>1.3870296199999999E-4</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1">
-        <v>1.6605117000000001E-4</v>
+        <v>1.4422597800000001E-2</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -9326,10 +10479,10 @@
         <v>1.2250734300000001E-4</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="F18" s="1">
-        <v>1.3685389499999999E-4</v>
+        <v>1.29375866E-2</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -9347,10 +10500,10 @@
         <v>1.17786181E-4</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1">
-        <v>1.3552866599999999E-4</v>
+        <v>1.29081903E-2</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -9368,10 +10521,10 @@
         <v>1.10919163E-4</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F20" s="1">
-        <v>1.2653776899999999E-4</v>
+        <v>1.2671995599999999E-2</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -9389,10 +10542,10 @@
         <v>1.0861653499999999E-4</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="F21" s="1">
-        <v>1.15241431E-4</v>
+        <v>1.2074678E-2</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -9410,10 +10563,10 @@
         <v>1.08039009E-4</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1">
-        <v>1.10354249E-4</v>
+        <v>1.20636571E-2</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -9431,10 +10584,10 @@
         <v>1.02342424E-4</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1">
-        <v>1.03855265E-4</v>
+        <v>1.1879538E-2</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -9452,10 +10605,10 @@
         <v>9.3380065300000003E-5</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="F24" s="1">
-        <v>1.0176904800000001E-4</v>
+        <v>1.1553381600000001E-2</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -9473,10 +10626,10 @@
         <v>9.0011028699999994E-5</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1">
-        <v>9.8218392599999996E-5</v>
+        <v>1.13898E-2</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -9494,10 +10647,10 @@
         <v>8.5312810399999994E-5</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F26" s="1">
-        <v>9.6296799599999996E-5</v>
+        <v>1.13727923E-2</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -9515,10 +10668,10 @@
         <v>8.3051561299999998E-5</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1">
-        <v>9.1799034899999997E-5</v>
+        <v>1.11576683E-2</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -9536,10 +10689,10 @@
         <v>8.20017516E-5</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F28" s="1">
-        <v>8.8631844600000004E-5</v>
+        <v>1.1062789199999999E-2</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -9557,10 +10710,10 @@
         <v>8.0906302300000002E-5</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F29" s="1">
-        <v>8.5614182099999993E-5</v>
+        <v>1.03199963E-2</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -9578,10 +10731,10 @@
         <v>7.83812684E-5</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="F30" s="1">
-        <v>8.0885469599999995E-5</v>
+        <v>9.9446641799999999E-3</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -9599,10 +10752,10 @@
         <v>7.35169089E-5</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F31" s="1">
-        <v>7.7394809599999994E-5</v>
+        <v>9.7167137800000004E-3</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -9620,10 +10773,10 @@
         <v>6.9079728900000003E-5</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F32" s="1">
-        <v>7.6279300300000001E-5</v>
+        <v>9.6578771000000001E-3</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -9641,10 +10794,10 @@
         <v>6.6486989800000005E-5</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1">
-        <v>7.1558080199999997E-5</v>
+        <v>8.7234240200000004E-3</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -9662,10 +10815,10 @@
         <v>6.3536800100000003E-5</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F34" s="1">
-        <v>6.9451634700000005E-5</v>
+        <v>8.6318010399999996E-3</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -9683,10 +10836,10 @@
         <v>6.1487819299999998E-5</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F35" s="1">
-        <v>6.8870900599999994E-5</v>
+        <v>8.6156411100000007E-3</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -9704,10 +10857,10 @@
         <v>6.0579933100000001E-5</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F36" s="1">
-        <v>6.4846736299999997E-5</v>
+        <v>8.61218253E-3</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -9725,10 +10878,10 @@
         <v>6.0480359499999997E-5</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F37" s="1">
-        <v>6.2991405300000003E-5</v>
+        <v>8.3742176800000005E-3</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -9746,10 +10899,10 @@
         <v>5.7479761600000001E-5</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F38" s="1">
-        <v>6.2464194300000002E-5</v>
+        <v>8.2916871699999992E-3</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -9767,10 +10920,10 @@
         <v>5.7157809400000001E-5</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="F39" s="1">
-        <v>6.1783204199999996E-5</v>
+        <v>8.1483840399999997E-3</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -9788,10 +10941,10 @@
         <v>5.6675246999999998E-5</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F40" s="1">
-        <v>6.1483818800000005E-5</v>
+        <v>8.1122279500000002E-3</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -9809,10 +10962,10 @@
         <v>5.59872968E-5</v>
       </c>
       <c r="E41" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F41" s="1">
-        <v>6.1383286900000005E-5</v>
+        <v>7.9079522999999999E-3</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -9830,10 +10983,10 @@
         <v>5.5808174999999997E-5</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="F42" s="1">
-        <v>6.09036798E-5</v>
+        <v>7.4428997E-3</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -9851,10 +11004,10 @@
         <v>5.5713743799999999E-5</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F43" s="1">
-        <v>5.9620771900000002E-5</v>
+        <v>7.2607542500000002E-3</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -9872,10 +11025,10 @@
         <v>5.5600129800000002E-5</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F44" s="1">
-        <v>5.6644420699999999E-5</v>
+        <v>7.0506677900000004E-3</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -9893,10 +11046,10 @@
         <v>5.3687147399999998E-5</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="F45" s="1">
-        <v>5.6536225299999999E-5</v>
+        <v>6.6078185100000002E-3</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -9914,10 +11067,10 @@
         <v>5.2301202200000002E-5</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F46" s="1">
-        <v>5.5665502800000003E-5</v>
+        <v>6.5493793700000004E-3</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -9935,10 +11088,10 @@
         <v>5.1137526999999997E-5</v>
       </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="F47" s="1">
-        <v>5.5626664700000003E-5</v>
+        <v>6.4394017399999996E-3</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -9956,10 +11109,10 @@
         <v>4.9284146799999997E-5</v>
       </c>
       <c r="E48" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F48" s="1">
-        <v>5.0841156999999999E-5</v>
+        <v>5.6009470300000001E-3</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -9977,10 +11130,10 @@
         <v>4.82633438E-5</v>
       </c>
       <c r="E49" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F49" s="1">
-        <v>4.9991532600000001E-5</v>
+        <v>5.4257679200000004E-3</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -9998,10 +11151,10 @@
         <v>4.70544796E-5</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F50" s="1">
-        <v>4.9336844099999997E-5</v>
+        <v>5.3857450399999998E-3</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -10019,10 +11172,10 @@
         <v>4.6688983E-5</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F51" s="1">
-        <v>4.92007335E-5</v>
+        <v>4.8479553199999997E-3</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -10040,10 +11193,10 @@
         <v>4.6328468499999999E-5</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="F52" s="1">
-        <v>4.88175435E-5</v>
+        <v>4.7746699200000003E-3</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -10061,10 +11214,10 @@
         <v>4.4265511700000003E-5</v>
       </c>
       <c r="E53" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F53" s="1">
-        <v>4.8358805299999997E-5</v>
+        <v>4.5794539400000004E-3</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -10082,10 +11235,10 @@
         <v>4.3532468999999999E-5</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F54" s="1">
-        <v>4.7456839000000003E-5</v>
+        <v>4.2988041200000002E-3</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -10106,7 +11259,7 @@
         <v>46</v>
       </c>
       <c r="F55" s="1">
-        <v>4.3773611300000002E-5</v>
+        <v>4.12321055E-3</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -10124,10 +11277,10 @@
         <v>3.7944449699999997E-5</v>
       </c>
       <c r="E56" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F56" s="1">
-        <v>4.0578043400000001E-5</v>
+        <v>3.6327386599999999E-3</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -10145,10 +11298,10 @@
         <v>3.7429067E-5</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F57" s="1">
-        <v>3.9919255899999997E-5</v>
+        <v>3.5338394499999999E-3</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -10166,10 +11319,10 @@
         <v>3.1804179200000002E-5</v>
       </c>
       <c r="E58" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="F58" s="1">
-        <v>3.8828314300000002E-5</v>
+        <v>3.4321147799999999E-3</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -10187,10 +11340,10 @@
         <v>2.9836405000000002E-5</v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F59" s="1">
-        <v>3.3549694600000002E-5</v>
+        <v>3.30297449E-3</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -10208,10 +11361,10 @@
         <v>2.4399308299999999E-5</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F60" s="1">
-        <v>3.0230107999999999E-5</v>
+        <v>3.2558153900000002E-3</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -10229,10 +11382,10 @@
         <v>2.35950108E-5</v>
       </c>
       <c r="E61" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F61" s="1">
-        <v>2.8373049000000002E-5</v>
+        <v>3.1657826199999999E-3</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -10250,10 +11403,10 @@
         <v>2.3034595299999999E-5</v>
       </c>
       <c r="E62" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F62" s="1">
-        <v>2.4751457499999999E-5</v>
+        <v>2.9440972100000001E-3</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -10271,10 +11424,10 @@
         <v>2.2832092500000001E-5</v>
       </c>
       <c r="E63" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F63" s="1">
-        <v>2.2791314400000001E-5</v>
+        <v>2.91751204E-3</v>
       </c>
       <c r="G63" s="1"/>
     </row>
@@ -10292,10 +11445,10 @@
         <v>1.8515246299999999E-5</v>
       </c>
       <c r="E64" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="F64" s="1">
-        <v>2.2170823099999999E-5</v>
+        <v>2.5420987200000002E-3</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -10313,10 +11466,10 @@
         <v>1.7227976199999999E-5</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F65" s="1">
-        <v>2.1151625000000001E-5</v>
+        <v>2.1550414900000001E-3</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -10334,10 +11487,10 @@
         <v>1.6698310500000001E-5</v>
       </c>
       <c r="E66" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F66" s="1">
-        <v>2.0848744399999999E-5</v>
+        <v>1.56710392E-3</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -10349,10 +11502,10 @@
         <v>1.5701056299999999E-5</v>
       </c>
       <c r="E67" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F67" s="1">
-        <v>1.84230585E-5</v>
+        <v>5.3064338699999999E-4</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -10363,10 +11516,10 @@
         <v>1.5588980600000001E-5</v>
       </c>
       <c r="E68" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F68" s="1">
-        <v>1.67734744E-5</v>
+        <v>5.8890088800000001E-5</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -10377,10 +11530,10 @@
         <v>9.9243465900000007E-7</v>
       </c>
       <c r="E69" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F69" s="1">
-        <v>9.8663581700000002E-7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10392,7 +11545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>

</xml_diff>